<commit_message>
Replaced more player numbers with names
</commit_message>
<xml_diff>
--- a/Strategies/strategy_custom_example.xlsx
+++ b/Strategies/strategy_custom_example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f4dee3fe07fcb0db/Documents/Georgia Tech/2021 Fall/ISyE6644/Blackjack Project/Strategies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0FDD4402-3420-43E1-A6C7-FEAECB866F3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{95EA3389-CB4A-4AEF-AE22-813C52E386BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5130" yWindow="3090" windowWidth="15390" windowHeight="9533" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hard" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="20">
   <si>
     <t>Player</t>
   </si>
@@ -81,7 +81,7 @@
     <t>SurrenderSplit</t>
   </si>
   <si>
-    <t>No Split</t>
+    <t>SplitH</t>
   </si>
 </sst>
 </file>
@@ -612,7 +612,70 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="38">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -623,7 +686,112 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="5" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1024,7 +1192,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="B18" sqref="B18:K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1696,16 +1864,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:K19">
-    <cfRule type="containsText" dxfId="13" priority="1" operator="containsText" text="Split">
+    <cfRule type="containsText" dxfId="37" priority="1" operator="containsText" text="Split">
       <formula>NOT(ISERROR(SEARCH("Split",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="2" operator="containsText" text="Double">
+    <cfRule type="containsText" dxfId="36" priority="2" operator="containsText" text="Double">
       <formula>NOT(ISERROR(SEARCH("Double",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="3" operator="containsText" text="Stand">
+    <cfRule type="containsText" dxfId="35" priority="3" operator="containsText" text="Stand">
       <formula>NOT(ISERROR(SEARCH("Stand",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="4" operator="containsText" text="Hit">
+    <cfRule type="containsText" dxfId="34" priority="4" operator="containsText" text="Hit">
       <formula>NOT(ISERROR(SEARCH("Hit",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1716,10 +1884,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1761,7 +1929,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -1770,13 +1938,13 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G2" t="s">
         <v>1</v>
@@ -1796,7 +1964,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -1831,7 +1999,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
@@ -1840,7 +2008,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4" t="s">
         <v>2</v>
@@ -1866,7 +2034,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
@@ -1901,13 +2069,13 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6" t="s">
         <v>2</v>
@@ -1936,28 +2104,28 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="F7" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="G7" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H7" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I7" t="s">
         <v>1</v>
@@ -1971,19 +2139,19 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="E8" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="F8" t="s">
         <v>16</v>
@@ -1995,63 +2163,134 @@
         <v>3</v>
       </c>
       <c r="I8" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K8" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" t="s">
+        <v>3</v>
+      </c>
+      <c r="H9" t="s">
+        <v>3</v>
+      </c>
+      <c r="I9" t="s">
+        <v>3</v>
+      </c>
+      <c r="J9" t="s">
+        <v>3</v>
+      </c>
+      <c r="K9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A10">
         <v>9</v>
       </c>
-      <c r="B9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E9" t="s">
-        <v>3</v>
-      </c>
-      <c r="F9" t="s">
-        <v>3</v>
-      </c>
-      <c r="G9" t="s">
-        <v>3</v>
-      </c>
-      <c r="H9" t="s">
-        <v>3</v>
-      </c>
-      <c r="I9" t="s">
-        <v>3</v>
-      </c>
-      <c r="J9" t="s">
-        <v>3</v>
-      </c>
-      <c r="K9" t="s">
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" t="s">
+        <v>3</v>
+      </c>
+      <c r="H10" t="s">
+        <v>3</v>
+      </c>
+      <c r="I10" t="s">
+        <v>3</v>
+      </c>
+      <c r="J10" t="s">
+        <v>3</v>
+      </c>
+      <c r="K10" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:K9">
-    <cfRule type="containsText" dxfId="9" priority="1" operator="containsText" text="Split">
-      <formula>NOT(ISERROR(SEARCH("Split",B2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="2" operator="containsText" text="Double">
-      <formula>NOT(ISERROR(SEARCH("Double",B2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="Stand">
-      <formula>NOT(ISERROR(SEARCH("Stand",B2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="Hit">
-      <formula>NOT(ISERROR(SEARCH("Hit",B2)))</formula>
+  <conditionalFormatting sqref="B3:K10">
+    <cfRule type="containsText" dxfId="33" priority="11" operator="containsText" text="Split">
+      <formula>NOT(ISERROR(SEARCH("Split",B3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="32" priority="12" operator="containsText" text="Double">
+      <formula>NOT(ISERROR(SEARCH("Double",B3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="31" priority="13" operator="containsText" text="Stand">
+      <formula>NOT(ISERROR(SEARCH("Stand",B3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="30" priority="14" operator="containsText" text="Hit">
+      <formula>NOT(ISERROR(SEARCH("Hit",B3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:C2 G2:XFD2">
+    <cfRule type="containsText" dxfId="29" priority="7" operator="containsText" text="Split">
+      <formula>NOT(ISERROR(SEARCH("Split",A2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="28" priority="8" operator="containsText" text="Double">
+      <formula>NOT(ISERROR(SEARCH("Double",A2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="27" priority="9" operator="containsText" text="Stand">
+      <formula>NOT(ISERROR(SEARCH("Stand",A2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="26" priority="10" operator="containsText" text="Hit">
+      <formula>NOT(ISERROR(SEARCH("Hit",A2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:C2 G2:XFD2">
+    <cfRule type="containsText" dxfId="25" priority="5" operator="containsText" text="No Split">
+      <formula>NOT(ISERROR(SEARCH("No Split",A2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="24" priority="6" operator="containsText" text="Surrender">
+      <formula>NOT(ISERROR(SEARCH("Surrender",A2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:F2">
+    <cfRule type="containsText" dxfId="23" priority="1" operator="containsText" text="Split">
+      <formula>NOT(ISERROR(SEARCH("Split",D2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="22" priority="2" operator="containsText" text="Double">
+      <formula>NOT(ISERROR(SEARCH("Double",D2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="21" priority="3" operator="containsText" text="Stand">
+      <formula>NOT(ISERROR(SEARCH("Stand",D2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="20" priority="4" operator="containsText" text="Hit">
+      <formula>NOT(ISERROR(SEARCH("Hit",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2062,8 +2301,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2108,10 +2347,10 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
         <v>17</v>
@@ -2143,10 +2382,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
         <v>17</v>
@@ -2187,10 +2426,10 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G4" t="s">
         <v>1</v>
@@ -2213,34 +2452,34 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="H5" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="I5" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="J5" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="K5" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.45">
@@ -2248,7 +2487,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
         <v>17</v>
@@ -2388,34 +2627,34 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="E10" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="F10" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="G10" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="H10" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="I10" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="J10" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="K10" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.45">
@@ -2454,26 +2693,76 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:K4 B6:K9 B11:K11">
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="Split">
+  <conditionalFormatting sqref="G2:K4 B7:K9 B11:K11 G6:K6">
+    <cfRule type="containsText" dxfId="19" priority="17" operator="containsText" text="Split">
       <formula>NOT(ISERROR(SEARCH("Split",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="Double">
+    <cfRule type="containsText" dxfId="18" priority="18" operator="containsText" text="Double">
       <formula>NOT(ISERROR(SEARCH("Double",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="Stand">
+    <cfRule type="containsText" dxfId="17" priority="19" operator="containsText" text="Stand">
       <formula>NOT(ISERROR(SEARCH("Stand",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="6" operator="containsText" text="Hit">
+    <cfRule type="containsText" dxfId="16" priority="20" operator="containsText" text="Hit">
       <formula>NOT(ISERROR(SEARCH("Hit",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:K11">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Surrender">
+  <conditionalFormatting sqref="B7:K9 G2:K4 G6:K6 B11:K11">
+    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="No Split">
+      <formula>NOT(ISERROR(SEARCH("No Split",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="14" priority="16" operator="containsText" text="Surrender">
       <formula>NOT(ISERROR(SEARCH("Surrender",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="No Split">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B6:F6 B2:F4">
+    <cfRule type="containsText" dxfId="13" priority="11" operator="containsText" text="Split">
+      <formula>NOT(ISERROR(SEARCH("Split",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="12" operator="containsText" text="Double">
+      <formula>NOT(ISERROR(SEARCH("Double",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="11" priority="13" operator="containsText" text="Stand">
+      <formula>NOT(ISERROR(SEARCH("Stand",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="14" operator="containsText" text="Hit">
+      <formula>NOT(ISERROR(SEARCH("Hit",B2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:F4 B6:F6">
+    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="No Split">
       <formula>NOT(ISERROR(SEARCH("No Split",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="Surrender">
+      <formula>NOT(ISERROR(SEARCH("Surrender",B2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5:K5">
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="Split">
+      <formula>NOT(ISERROR(SEARCH("Split",B5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="Double">
+      <formula>NOT(ISERROR(SEARCH("Double",B5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="Stand">
+      <formula>NOT(ISERROR(SEARCH("Stand",B5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="Hit">
+      <formula>NOT(ISERROR(SEARCH("Hit",B5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B10:K10">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Split">
+      <formula>NOT(ISERROR(SEARCH("Split",B10)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Double">
+      <formula>NOT(ISERROR(SEARCH("Double",B10)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="Stand">
+      <formula>NOT(ISERROR(SEARCH("Stand",B10)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="Hit">
+      <formula>NOT(ISERROR(SEARCH("Hit",B10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>